<commit_message>
updates polind posa e olio
</commit_message>
<xml_diff>
--- a/data-raw/polifenoli/2020/polifenoli_HPLC_olio.xlsx
+++ b/data-raw/polifenoli/2020/polifenoli_HPLC_olio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\Desktop\file progetto\polifenoli veri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03D6163-B262-4701-AE6B-39B12021032B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FA6533-17E4-41A8-8064-BD1A43953E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D42F1501-9FEC-4851-B7BD-B10C81F9B577}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="25275" windowHeight="13755" xr2:uid="{D42F1501-9FEC-4851-B7BD-B10C81F9B577}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="44">
   <si>
     <t>Idrossitirosolo</t>
   </si>
@@ -160,6 +160,15 @@
   </si>
   <si>
     <t>R2</t>
+  </si>
+  <si>
+    <t>SA_03</t>
+  </si>
+  <si>
+    <t>NA_02</t>
+  </si>
+  <si>
+    <t>CE_02</t>
   </si>
 </sst>
 </file>
@@ -201,8 +210,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -517,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{515717C1-F799-4246-BFAC-63AB3ABCF04F}">
-  <dimension ref="A1:O64"/>
+  <dimension ref="A1:O73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,25 +623,25 @@
         <v>2</v>
       </c>
       <c r="I2">
-        <v>0.2495</v>
+        <v>249.5</v>
       </c>
       <c r="J2">
-        <v>4.5359999999999998E-2</v>
+        <v>45.36</v>
       </c>
       <c r="K2">
-        <v>3.0299999999999997E-3</v>
+        <v>3.03</v>
       </c>
       <c r="L2">
-        <v>1.3640000000000002E-3</v>
+        <v>1.3640000000000001</v>
       </c>
       <c r="M2">
-        <v>1.0182999999999999E-2</v>
+        <v>10.183</v>
       </c>
       <c r="N2">
-        <v>6.1785E-2</v>
+        <v>61.784999999999997</v>
       </c>
       <c r="O2">
-        <v>9.8820000000000002E-3</v>
+        <v>9.8819999999999997</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -660,25 +670,25 @@
         <v>2</v>
       </c>
       <c r="I3">
-        <v>0.25014999999999998</v>
+        <v>250.15</v>
       </c>
       <c r="J3">
-        <v>4.5869999999999994E-2</v>
+        <v>45.87</v>
       </c>
       <c r="K3">
-        <v>2.98E-3</v>
+        <v>2.98</v>
       </c>
       <c r="L3">
-        <v>1.2980000000000001E-3</v>
+        <v>1.298</v>
       </c>
       <c r="M3">
-        <v>1.0994E-2</v>
+        <v>10.994</v>
       </c>
       <c r="N3">
-        <v>5.9878999999999995E-2</v>
+        <v>59.878999999999998</v>
       </c>
       <c r="O3">
-        <v>8.5210000000000008E-3</v>
+        <v>8.5210000000000008</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -707,25 +717,25 @@
         <v>2</v>
       </c>
       <c r="I4">
-        <v>0.24987000000000001</v>
+        <v>249.87</v>
       </c>
       <c r="J4">
-        <v>4.6240000000000003E-2</v>
+        <v>46.24</v>
       </c>
       <c r="K4">
-        <v>2.8700000000000002E-3</v>
+        <v>2.87</v>
       </c>
       <c r="L4">
-        <v>1.4419999999999999E-3</v>
+        <v>1.4419999999999999</v>
       </c>
       <c r="M4">
-        <v>8.9969999999999998E-3</v>
+        <v>8.9969999999999999</v>
       </c>
       <c r="N4">
-        <v>6.3213999999999992E-2</v>
+        <v>63.213999999999999</v>
       </c>
       <c r="O4">
-        <v>9.2650000000000007E-3</v>
+        <v>9.2650000000000006</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -754,25 +764,25 @@
         <v>2</v>
       </c>
       <c r="I5">
-        <v>0.21832699999999999</v>
+        <v>218.327</v>
       </c>
       <c r="J5">
-        <v>3.3182000000000003E-2</v>
+        <v>33.182000000000002</v>
       </c>
       <c r="K5">
-        <v>9.9099999999999991E-4</v>
+        <v>0.99099999999999999</v>
       </c>
       <c r="L5">
-        <v>7.6199999999999998E-4</v>
+        <v>0.76200000000000001</v>
       </c>
       <c r="M5">
-        <v>4.0051000000000003E-2</v>
+        <v>40.051000000000002</v>
       </c>
       <c r="N5">
-        <v>0.22792899999999999</v>
+        <v>227.929</v>
       </c>
       <c r="O5">
-        <v>8.7819999999999999E-3</v>
+        <v>8.782</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -801,25 +811,25 @@
         <v>2</v>
       </c>
       <c r="I6">
-        <v>0.21235400000000001</v>
+        <v>212.35400000000001</v>
       </c>
       <c r="J6">
-        <v>2.9870000000000001E-2</v>
+        <v>29.87</v>
       </c>
       <c r="K6">
-        <v>1.1200000000000001E-3</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="L6">
-        <v>8.7500000000000002E-4</v>
+        <v>0.875</v>
       </c>
       <c r="M6">
-        <v>3.9884999999999997E-2</v>
+        <v>39.884999999999998</v>
       </c>
       <c r="N6">
-        <v>0.20155999999999999</v>
+        <v>201.56</v>
       </c>
       <c r="O6">
-        <v>6.9870000000000002E-3</v>
+        <v>6.9870000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -848,25 +858,25 @@
         <v>2</v>
       </c>
       <c r="I7">
-        <v>0.21958000000000003</v>
+        <v>219.58</v>
       </c>
       <c r="J7">
-        <v>3.5673999999999997E-2</v>
+        <v>35.673999999999999</v>
       </c>
       <c r="K7">
-        <v>1.0149999999999998E-3</v>
+        <v>1.0149999999999999</v>
       </c>
       <c r="L7">
-        <v>6.4999999999999997E-4</v>
+        <v>0.65</v>
       </c>
       <c r="M7">
-        <v>4.1229999999999996E-2</v>
+        <v>41.23</v>
       </c>
       <c r="N7">
-        <v>0.237568</v>
+        <v>237.56800000000001</v>
       </c>
       <c r="O7">
-        <v>9.9869999999999994E-3</v>
+        <v>9.9870000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -895,25 +905,25 @@
         <v>2</v>
       </c>
       <c r="I8">
-        <v>0.196052</v>
+        <v>196.05199999999999</v>
       </c>
       <c r="J8">
-        <v>4.2315999999999999E-2</v>
+        <v>42.316000000000003</v>
       </c>
       <c r="K8">
-        <v>1.3309999999999999E-3</v>
+        <v>1.331</v>
       </c>
       <c r="L8">
-        <v>7.4299999999999995E-4</v>
+        <v>0.74299999999999999</v>
       </c>
       <c r="M8">
-        <v>4.7084000000000001E-2</v>
+        <v>47.084000000000003</v>
       </c>
       <c r="N8">
-        <v>0.27729300000000001</v>
+        <v>277.29300000000001</v>
       </c>
       <c r="O8">
-        <v>7.0140000000000003E-3</v>
+        <v>7.0140000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -942,25 +952,25 @@
         <v>2</v>
       </c>
       <c r="I9">
-        <v>0.21029499999999998</v>
+        <v>210.29499999999999</v>
       </c>
       <c r="J9">
-        <v>4.3156E-2</v>
+        <v>43.155999999999999</v>
       </c>
       <c r="K9">
-        <v>7.7800000000000005E-4</v>
+        <v>0.77800000000000002</v>
       </c>
       <c r="L9">
-        <v>1.2600000000000001E-3</v>
+        <v>1.26</v>
       </c>
       <c r="M9">
-        <v>4.5259999999999995E-2</v>
+        <v>45.26</v>
       </c>
       <c r="N9">
-        <v>0.28764999999999996</v>
+        <v>287.64999999999998</v>
       </c>
       <c r="O9">
-        <v>5.2129999999999998E-3</v>
+        <v>5.2130000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -989,25 +999,25 @@
         <v>2</v>
       </c>
       <c r="I10">
-        <v>0.20014999999999999</v>
+        <v>200.15</v>
       </c>
       <c r="J10">
-        <v>3.9869999999999996E-2</v>
+        <v>39.869999999999997</v>
       </c>
       <c r="K10">
-        <v>9.7999999999999997E-4</v>
+        <v>0.98</v>
       </c>
       <c r="L10">
-        <v>1.1020000000000001E-3</v>
+        <v>1.1020000000000001</v>
       </c>
       <c r="M10">
-        <v>3.875E-2</v>
+        <v>38.75</v>
       </c>
       <c r="N10">
-        <v>0.21568000000000001</v>
+        <v>215.68</v>
       </c>
       <c r="O10">
-        <v>8.4979999999999986E-3</v>
+        <v>8.4979999999999993</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -1039,19 +1049,19 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>5.2937999999999999E-2</v>
+        <v>52.938000000000002</v>
       </c>
       <c r="K11">
-        <v>2.8929999999999997E-3</v>
+        <v>2.8929999999999998</v>
       </c>
       <c r="L11">
-        <v>7.1699999999999997E-4</v>
+        <v>0.71699999999999997</v>
       </c>
       <c r="M11">
-        <v>4.4340000000000004E-3</v>
+        <v>4.4340000000000002</v>
       </c>
       <c r="N11">
-        <v>6.6096999999999989E-2</v>
+        <v>66.096999999999994</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -1086,22 +1096,22 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>5.1679999999999997E-2</v>
+        <v>51.68</v>
       </c>
       <c r="K12">
-        <v>1.9989999999999999E-3</v>
+        <v>1.9990000000000001</v>
       </c>
       <c r="L12">
-        <v>8.7500000000000002E-4</v>
+        <v>0.875</v>
       </c>
       <c r="M12">
-        <v>2.9809999999999997E-3</v>
+        <v>2.9809999999999999</v>
       </c>
       <c r="N12">
-        <v>6.6269999999999996E-2</v>
+        <v>66.27</v>
       </c>
       <c r="O12">
-        <v>1.1999999999999999E-4</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -1133,19 +1143,19 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <v>5.5210000000000002E-2</v>
+        <v>55.21</v>
       </c>
       <c r="K13">
-        <v>3.5699999999999998E-3</v>
+        <v>3.57</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13">
-        <v>4.8920000000000005E-3</v>
+        <v>4.8920000000000003</v>
       </c>
       <c r="N13">
-        <v>6.4588999999999994E-2</v>
+        <v>64.588999999999999</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -1177,25 +1187,25 @@
         <v>2</v>
       </c>
       <c r="I14">
-        <v>1.2598000000000002E-2</v>
+        <v>12.598000000000001</v>
       </c>
       <c r="J14">
-        <v>5.6515000000000003E-2</v>
+        <v>56.515000000000001</v>
       </c>
       <c r="K14">
-        <v>4.0860000000000002E-3</v>
+        <v>4.0860000000000003</v>
       </c>
       <c r="L14">
-        <v>1.219E-3</v>
+        <v>1.2190000000000001</v>
       </c>
       <c r="M14">
-        <v>9.2820000000000003E-3</v>
+        <v>9.282</v>
       </c>
       <c r="N14">
-        <v>0.15537399999999998</v>
+        <v>155.374</v>
       </c>
       <c r="O14">
-        <v>3.5249999999999999E-3</v>
+        <v>3.5249999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -1224,25 +1234,25 @@
         <v>2</v>
       </c>
       <c r="I15">
-        <v>1.0987E-2</v>
+        <v>10.987</v>
       </c>
       <c r="J15">
-        <v>5.5458E-2</v>
+        <v>55.457999999999998</v>
       </c>
       <c r="K15">
-        <v>4.4589999999999994E-3</v>
+        <v>4.4589999999999996</v>
       </c>
       <c r="L15">
-        <v>1.598E-3</v>
+        <v>1.5980000000000001</v>
       </c>
       <c r="M15">
-        <v>8.9979999999999991E-3</v>
+        <v>8.9979999999999993</v>
       </c>
       <c r="N15">
-        <v>0.150258</v>
+        <v>150.25800000000001</v>
       </c>
       <c r="O15">
-        <v>2.98E-3</v>
+        <v>2.98</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -1271,25 +1281,25 @@
         <v>2</v>
       </c>
       <c r="I16">
-        <v>1.2215E-2</v>
+        <v>12.215</v>
       </c>
       <c r="J16">
-        <v>5.5999E-2</v>
+        <v>55.999000000000002</v>
       </c>
       <c r="K16">
-        <v>2.98E-3</v>
+        <v>2.98</v>
       </c>
       <c r="L16">
-        <v>1.3209999999999999E-3</v>
+        <v>1.321</v>
       </c>
       <c r="M16">
-        <v>9.11E-3</v>
+        <v>9.11</v>
       </c>
       <c r="N16">
-        <v>0.15867300000000001</v>
+        <v>158.673</v>
       </c>
       <c r="O16">
-        <v>3.6240000000000001E-3</v>
+        <v>3.6240000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -1317,26 +1327,26 @@
       <c r="H17">
         <v>2</v>
       </c>
-      <c r="I17">
-        <v>0.24038399999999999</v>
-      </c>
-      <c r="J17">
-        <v>3.7814999999999994E-2</v>
-      </c>
-      <c r="K17">
-        <v>3.2589999999999997E-3</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17">
-        <v>1.0199E-2</v>
-      </c>
-      <c r="N17">
-        <v>5.8758000000000005E-2</v>
-      </c>
-      <c r="O17">
-        <v>6.13E-3</v>
+      <c r="I17" s="1">
+        <v>240.38399999999999</v>
+      </c>
+      <c r="J17" s="1">
+        <v>37.814999999999998</v>
+      </c>
+      <c r="K17" s="1">
+        <v>3.2589999999999999</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0</v>
+      </c>
+      <c r="M17" s="1">
+        <v>10.199</v>
+      </c>
+      <c r="N17" s="1">
+        <v>58.758000000000003</v>
+      </c>
+      <c r="O17" s="1">
+        <v>6.13</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -1364,26 +1374,26 @@
       <c r="H18">
         <v>2</v>
       </c>
-      <c r="I18">
-        <v>0.23587</v>
-      </c>
-      <c r="J18">
-        <v>3.5479999999999998E-2</v>
-      </c>
-      <c r="K18">
-        <v>2.8900000000000002E-3</v>
-      </c>
-      <c r="L18">
-        <v>1.26E-4</v>
-      </c>
-      <c r="M18">
-        <v>8.7889999999999999E-3</v>
-      </c>
-      <c r="N18">
-        <v>5.8168999999999998E-2</v>
-      </c>
-      <c r="O18">
-        <v>5.1600000000000005E-3</v>
+      <c r="I18" s="1">
+        <v>235.87</v>
+      </c>
+      <c r="J18" s="1">
+        <v>35.479999999999997</v>
+      </c>
+      <c r="K18" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0.126</v>
+      </c>
+      <c r="M18" s="1">
+        <v>8.7889999999999997</v>
+      </c>
+      <c r="N18" s="1">
+        <v>58.168999999999997</v>
+      </c>
+      <c r="O18" s="1">
+        <v>5.16</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -1411,26 +1421,26 @@
       <c r="H19">
         <v>2</v>
       </c>
-      <c r="I19">
-        <v>0.20128000000000001</v>
-      </c>
-      <c r="J19">
-        <v>3.6569999999999998E-2</v>
-      </c>
-      <c r="K19">
-        <v>3.1520000000000003E-3</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <v>8.9990000000000001E-3</v>
-      </c>
-      <c r="N19">
-        <v>5.7887999999999995E-2</v>
-      </c>
-      <c r="O19">
-        <v>6.0099999999999997E-3</v>
+      <c r="I19" s="1">
+        <v>201.28</v>
+      </c>
+      <c r="J19" s="1">
+        <v>36.57</v>
+      </c>
+      <c r="K19" s="1">
+        <v>3.1520000000000001</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0</v>
+      </c>
+      <c r="M19" s="1">
+        <v>8.9990000000000006</v>
+      </c>
+      <c r="N19" s="1">
+        <v>57.887999999999998</v>
+      </c>
+      <c r="O19" s="1">
+        <v>6.01</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1458,26 +1468,26 @@
       <c r="H20">
         <v>2</v>
       </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>4.9036000000000003E-2</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>7.0599999999999992E-4</v>
-      </c>
-      <c r="M20">
-        <v>5.8460000000000005E-3</v>
-      </c>
-      <c r="N20">
-        <v>0.119726</v>
-      </c>
-      <c r="O20">
-        <v>3.4710000000000001E-3</v>
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
+      <c r="J20" s="1">
+        <v>49.036000000000001</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="M20" s="1">
+        <v>5.8460000000000001</v>
+      </c>
+      <c r="N20" s="1">
+        <v>119.726</v>
+      </c>
+      <c r="O20" s="1">
+        <v>3.4710000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -1505,26 +1515,26 @@
       <c r="H21">
         <v>2</v>
       </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <v>4.9509999999999998E-2</v>
-      </c>
-      <c r="K21">
-        <v>1.25E-4</v>
-      </c>
-      <c r="L21">
-        <v>9.8700000000000003E-4</v>
-      </c>
-      <c r="M21">
-        <v>4.9870000000000001E-3</v>
-      </c>
-      <c r="N21">
-        <v>0.108596</v>
-      </c>
-      <c r="O21">
-        <v>2.9870000000000001E-3</v>
+      <c r="I21" s="1">
+        <v>0</v>
+      </c>
+      <c r="J21" s="1">
+        <v>49.51</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0.125</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="M21" s="1">
+        <v>4.9870000000000001</v>
+      </c>
+      <c r="N21" s="1">
+        <v>108.596</v>
+      </c>
+      <c r="O21" s="1">
+        <v>2.9870000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -1552,26 +1562,26 @@
       <c r="H22">
         <v>2</v>
       </c>
-      <c r="I22">
-        <v>3.5799999999999997E-4</v>
-      </c>
-      <c r="J22">
-        <v>5.2150000000000002E-2</v>
-      </c>
-      <c r="K22">
-        <v>1.1E-4</v>
-      </c>
-      <c r="L22">
-        <v>7.7800000000000005E-4</v>
-      </c>
-      <c r="M22">
-        <v>5.9870000000000001E-3</v>
-      </c>
-      <c r="N22">
-        <v>0.12015000000000001</v>
-      </c>
-      <c r="O22">
-        <v>3.4580000000000001E-3</v>
+      <c r="I22" s="1">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="J22" s="1">
+        <v>52.15</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="L22" s="1">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="M22" s="1">
+        <v>5.9870000000000001</v>
+      </c>
+      <c r="N22" s="1">
+        <v>120.15</v>
+      </c>
+      <c r="O22" s="1">
+        <v>3.4580000000000002</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -1599,26 +1609,26 @@
       <c r="H23">
         <v>2</v>
       </c>
-      <c r="I23">
-        <v>0.19204300000000002</v>
-      </c>
-      <c r="J23">
-        <v>4.2424999999999997E-2</v>
-      </c>
-      <c r="K23">
-        <v>3.2759999999999998E-3</v>
-      </c>
-      <c r="L23">
-        <v>9.3799999999999992E-4</v>
-      </c>
-      <c r="M23">
-        <v>1.1031000000000001E-2</v>
-      </c>
-      <c r="N23">
-        <v>6.3460000000000003E-2</v>
-      </c>
-      <c r="O23">
-        <v>2.856E-3</v>
+      <c r="I23" s="1">
+        <v>192.04300000000001</v>
+      </c>
+      <c r="J23" s="1">
+        <v>42.424999999999997</v>
+      </c>
+      <c r="K23" s="1">
+        <v>3.2759999999999998</v>
+      </c>
+      <c r="L23" s="1">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="M23" s="1">
+        <v>11.031000000000001</v>
+      </c>
+      <c r="N23" s="1">
+        <v>63.46</v>
+      </c>
+      <c r="O23" s="1">
+        <v>2.8559999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -1646,26 +1656,26 @@
       <c r="H24">
         <v>2</v>
       </c>
-      <c r="I24">
-        <v>0.19025</v>
-      </c>
-      <c r="J24">
-        <v>4.4119999999999999E-2</v>
-      </c>
-      <c r="K24">
-        <v>2.8900000000000002E-3</v>
-      </c>
-      <c r="L24">
-        <v>7.9799999999999999E-4</v>
-      </c>
-      <c r="M24">
-        <v>1.0987E-2</v>
-      </c>
-      <c r="N24">
-        <v>6.1249999999999999E-2</v>
-      </c>
-      <c r="O24">
-        <v>2.6800000000000001E-3</v>
+      <c r="I24" s="1">
+        <v>190.25</v>
+      </c>
+      <c r="J24" s="1">
+        <v>44.12</v>
+      </c>
+      <c r="K24" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="L24" s="1">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="M24" s="1">
+        <v>10.987</v>
+      </c>
+      <c r="N24" s="1">
+        <v>61.25</v>
+      </c>
+      <c r="O24" s="1">
+        <v>2.68</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -1693,26 +1703,26 @@
       <c r="H25">
         <v>2</v>
       </c>
-      <c r="I25">
-        <v>0.19125</v>
-      </c>
-      <c r="J25">
-        <v>4.3158000000000002E-2</v>
-      </c>
-      <c r="K25">
-        <v>3.0099999999999997E-3</v>
-      </c>
-      <c r="L25">
-        <v>8.7000000000000001E-4</v>
-      </c>
-      <c r="M25">
-        <v>9.0139999999999994E-3</v>
-      </c>
-      <c r="N25">
-        <v>6.4569999999999989E-2</v>
-      </c>
-      <c r="O25">
-        <v>2.5699999999999998E-3</v>
+      <c r="I25" s="1">
+        <v>191.25</v>
+      </c>
+      <c r="J25" s="1">
+        <v>43.158000000000001</v>
+      </c>
+      <c r="K25" s="1">
+        <v>3.01</v>
+      </c>
+      <c r="L25" s="1">
+        <v>0.87</v>
+      </c>
+      <c r="M25" s="1">
+        <v>9.0139999999999993</v>
+      </c>
+      <c r="N25" s="1">
+        <v>64.569999999999993</v>
+      </c>
+      <c r="O25" s="1">
+        <v>2.57</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -1740,25 +1750,25 @@
       <c r="H26">
         <v>2</v>
       </c>
-      <c r="I26">
-        <v>1.6989999999999998E-2</v>
-      </c>
-      <c r="J26">
-        <v>4.4296999999999996E-2</v>
-      </c>
-      <c r="K26">
-        <v>3.8509999999999998E-3</v>
-      </c>
-      <c r="L26">
-        <v>0</v>
-      </c>
-      <c r="M26">
-        <v>7.2249999999999997E-3</v>
-      </c>
-      <c r="N26">
-        <v>0.14200299999999999</v>
-      </c>
-      <c r="O26">
+      <c r="I26" s="1">
+        <v>16.989999999999998</v>
+      </c>
+      <c r="J26" s="1">
+        <v>44.296999999999997</v>
+      </c>
+      <c r="K26" s="1">
+        <v>3.851</v>
+      </c>
+      <c r="L26" s="1">
+        <v>0</v>
+      </c>
+      <c r="M26" s="1">
+        <v>7.2249999999999996</v>
+      </c>
+      <c r="N26" s="1">
+        <v>142.00299999999999</v>
+      </c>
+      <c r="O26" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1787,26 +1797,26 @@
       <c r="H27">
         <v>2</v>
       </c>
-      <c r="I27">
-        <v>1.7852E-2</v>
-      </c>
-      <c r="J27">
-        <v>4.4875999999999999E-2</v>
-      </c>
-      <c r="K27">
-        <v>3.5479999999999999E-3</v>
-      </c>
-      <c r="L27">
-        <v>2.22E-4</v>
-      </c>
-      <c r="M27">
-        <v>7.3540000000000003E-3</v>
-      </c>
-      <c r="N27">
-        <v>0.14498</v>
-      </c>
-      <c r="O27">
-        <v>1.1899999999999999E-4</v>
+      <c r="I27" s="1">
+        <v>17.852</v>
+      </c>
+      <c r="J27" s="1">
+        <v>44.875999999999998</v>
+      </c>
+      <c r="K27" s="1">
+        <v>3.548</v>
+      </c>
+      <c r="L27" s="1">
+        <v>0.222</v>
+      </c>
+      <c r="M27" s="1">
+        <v>7.3540000000000001</v>
+      </c>
+      <c r="N27" s="1">
+        <v>144.97999999999999</v>
+      </c>
+      <c r="O27" s="1">
+        <v>0.11899999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -1834,26 +1844,26 @@
       <c r="H28">
         <v>2</v>
       </c>
-      <c r="I28">
-        <v>1.6587000000000001E-2</v>
-      </c>
-      <c r="J28">
-        <v>4.2167999999999997E-2</v>
-      </c>
-      <c r="K28">
-        <v>4.1589999999999995E-3</v>
-      </c>
-      <c r="L28">
-        <v>5.9699999999999998E-4</v>
-      </c>
-      <c r="M28">
-        <v>6.28E-3</v>
-      </c>
-      <c r="N28">
-        <v>0.14388999999999999</v>
-      </c>
-      <c r="O28">
-        <v>2.0999999999999998E-4</v>
+      <c r="I28" s="1">
+        <v>16.587</v>
+      </c>
+      <c r="J28" s="1">
+        <v>42.167999999999999</v>
+      </c>
+      <c r="K28" s="1">
+        <v>4.1589999999999998</v>
+      </c>
+      <c r="L28" s="1">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="M28" s="1">
+        <v>6.28</v>
+      </c>
+      <c r="N28" s="1">
+        <v>143.88999999999999</v>
+      </c>
+      <c r="O28" s="1">
+        <v>0.21</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -1885,19 +1895,19 @@
         <v>0</v>
       </c>
       <c r="J29">
-        <v>6.5670000000000006E-2</v>
+        <v>65.67</v>
       </c>
       <c r="K29">
         <v>0</v>
       </c>
       <c r="L29">
-        <v>1.5229999999999998E-3</v>
+        <v>1.5229999999999999</v>
       </c>
       <c r="M29">
-        <v>3.055E-3</v>
+        <v>3.0550000000000002</v>
       </c>
       <c r="N29">
-        <v>2.9708999999999999E-2</v>
+        <v>29.709</v>
       </c>
       <c r="O29">
         <v>0</v>
@@ -1929,25 +1939,25 @@
         <v>2</v>
       </c>
       <c r="I30">
-        <v>2.5000000000000001E-4</v>
+        <v>0.25</v>
       </c>
       <c r="J30">
-        <v>6.3987000000000002E-2</v>
+        <v>63.987000000000002</v>
       </c>
       <c r="K30">
-        <v>2.9799999999999998E-4</v>
+        <v>0.29799999999999999</v>
       </c>
       <c r="L30">
-        <v>1.5969999999999999E-3</v>
+        <v>1.597</v>
       </c>
       <c r="M30">
-        <v>3.2400000000000003E-3</v>
+        <v>3.24</v>
       </c>
       <c r="N30">
-        <v>2.8797999999999997E-2</v>
+        <v>28.797999999999998</v>
       </c>
       <c r="O30">
-        <v>5.2400000000000005E-4</v>
+        <v>0.52400000000000002</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -1976,30 +1986,30 @@
         <v>2</v>
       </c>
       <c r="I31">
-        <v>5.9800000000000001E-4</v>
+        <v>0.59799999999999998</v>
       </c>
       <c r="J31">
-        <v>6.6244999999999998E-2</v>
+        <v>66.245000000000005</v>
       </c>
       <c r="K31">
-        <v>1.1249999999999999E-3</v>
+        <v>1.125</v>
       </c>
       <c r="L31">
-        <v>9.9700000000000006E-4</v>
+        <v>0.997</v>
       </c>
       <c r="M31">
-        <v>2.9870000000000001E-3</v>
+        <v>2.9870000000000001</v>
       </c>
       <c r="N31">
-        <v>2.7892E-2</v>
+        <v>27.891999999999999</v>
       </c>
       <c r="O31">
-        <v>1.1259999999999998E-3</v>
+        <v>1.1259999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="B32" t="s">
         <v>40</v>
@@ -2017,28 +2027,28 @@
         <v>1</v>
       </c>
       <c r="G32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I32">
-        <v>5.6375999999999996E-2</v>
+        <v>7.5380000000000003</v>
       </c>
       <c r="J32">
-        <v>0.31168299999999999</v>
+        <v>59.798000000000002</v>
       </c>
       <c r="K32">
         <v>0</v>
       </c>
       <c r="L32">
-        <v>7.5780000000000005E-3</v>
+        <v>3.427</v>
       </c>
       <c r="M32">
-        <v>9.2880000000000011E-3</v>
+        <v>9.8130000000000006</v>
       </c>
       <c r="N32">
-        <v>2.9748E-2</v>
+        <v>41.863</v>
       </c>
       <c r="O32">
         <v>0</v>
@@ -2046,7 +2056,7 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="B33" t="s">
         <v>40</v>
@@ -2064,36 +2074,36 @@
         <v>1</v>
       </c>
       <c r="G33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I33">
-        <v>5.3671999999999997E-2</v>
+        <v>6.9850000000000003</v>
       </c>
       <c r="J33">
-        <v>0.31524000000000002</v>
+        <v>60.256</v>
       </c>
       <c r="K33">
-        <v>9.8499999999999998E-4</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="L33">
-        <v>7.4229999999999999E-3</v>
+        <v>2.9870000000000001</v>
       </c>
       <c r="M33">
-        <v>5.6779999999999999E-3</v>
+        <v>8.7560000000000002</v>
       </c>
       <c r="N33">
-        <v>3.1251000000000001E-2</v>
+        <v>42.698</v>
       </c>
       <c r="O33">
-        <v>3.68E-4</v>
+        <v>1.24</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="B34" t="s">
         <v>40</v>
@@ -2111,36 +2121,36 @@
         <v>1</v>
       </c>
       <c r="G34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I34">
-        <v>5.8654999999999999E-2</v>
+        <v>7.1230000000000002</v>
       </c>
       <c r="J34">
-        <v>0.30986999999999998</v>
+        <v>59.987000000000002</v>
       </c>
       <c r="K34">
-        <v>2.43E-4</v>
+        <v>0.214</v>
       </c>
       <c r="L34">
-        <v>6.2449999999999997E-3</v>
+        <v>4.1260000000000003</v>
       </c>
       <c r="M34">
-        <v>7.8899999999999994E-3</v>
+        <v>9.5259999999999998</v>
       </c>
       <c r="N34">
-        <v>3.0254E-2</v>
+        <v>44.258000000000003</v>
       </c>
       <c r="O34">
-        <v>1.24E-3</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B35" t="s">
         <v>40</v>
@@ -2163,31 +2173,31 @@
       <c r="H35">
         <v>2</v>
       </c>
-      <c r="I35">
-        <v>4.2347999999999997E-2</v>
-      </c>
-      <c r="J35">
-        <v>6.9569999999999993E-2</v>
-      </c>
-      <c r="K35">
-        <v>1.6439999999999998E-3</v>
-      </c>
-      <c r="L35">
-        <v>1.1439999999999998E-3</v>
-      </c>
-      <c r="M35">
-        <v>9.469E-3</v>
-      </c>
-      <c r="N35">
-        <v>5.9847000000000004E-2</v>
-      </c>
-      <c r="O35">
+      <c r="I35" s="1">
+        <v>56.375999999999998</v>
+      </c>
+      <c r="J35" s="1">
+        <v>311.68299999999999</v>
+      </c>
+      <c r="K35" s="1">
+        <v>0</v>
+      </c>
+      <c r="L35" s="1">
+        <v>7.5780000000000003</v>
+      </c>
+      <c r="M35" s="1">
+        <v>9.2880000000000003</v>
+      </c>
+      <c r="N35" s="1">
+        <v>29.748000000000001</v>
+      </c>
+      <c r="O35" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B36" t="s">
         <v>40</v>
@@ -2210,31 +2220,31 @@
       <c r="H36">
         <v>2</v>
       </c>
-      <c r="I36">
-        <v>4.4234999999999997E-2</v>
-      </c>
-      <c r="J36">
-        <v>6.6678000000000001E-2</v>
-      </c>
-      <c r="K36">
-        <v>1.2669999999999999E-3</v>
-      </c>
-      <c r="L36">
-        <v>1.098E-3</v>
-      </c>
-      <c r="M36">
-        <v>8.967000000000001E-3</v>
-      </c>
-      <c r="N36">
-        <v>6.6577999999999998E-2</v>
-      </c>
-      <c r="O36">
-        <v>1E-4</v>
+      <c r="I36" s="1">
+        <v>53.671999999999997</v>
+      </c>
+      <c r="J36" s="1">
+        <v>315.24</v>
+      </c>
+      <c r="K36" s="1">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="L36" s="1">
+        <v>7.423</v>
+      </c>
+      <c r="M36" s="1">
+        <v>5.6779999999999999</v>
+      </c>
+      <c r="N36" s="1">
+        <v>31.251000000000001</v>
+      </c>
+      <c r="O36" s="1">
+        <v>0.36799999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B37" t="s">
         <v>40</v>
@@ -2257,31 +2267,31 @@
       <c r="H37">
         <v>2</v>
       </c>
-      <c r="I37">
-        <v>3.9578000000000002E-2</v>
-      </c>
-      <c r="J37">
-        <v>7.2650000000000006E-2</v>
-      </c>
-      <c r="K37">
-        <v>1.3500000000000001E-3</v>
-      </c>
-      <c r="L37">
-        <v>1.2669999999999999E-3</v>
-      </c>
-      <c r="M37">
-        <v>8.6639999999999998E-3</v>
-      </c>
-      <c r="N37">
-        <v>6.2354E-2</v>
-      </c>
-      <c r="O37">
-        <v>8.9999999999999992E-5</v>
+      <c r="I37" s="1">
+        <v>58.655000000000001</v>
+      </c>
+      <c r="J37" s="1">
+        <v>309.87</v>
+      </c>
+      <c r="K37" s="1">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="L37" s="1">
+        <v>6.2450000000000001</v>
+      </c>
+      <c r="M37" s="1">
+        <v>7.89</v>
+      </c>
+      <c r="N37" s="1">
+        <v>30.254000000000001</v>
+      </c>
+      <c r="O37" s="1">
+        <v>1.24</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B38" t="s">
         <v>40</v>
@@ -2304,31 +2314,31 @@
       <c r="H38">
         <v>2</v>
       </c>
-      <c r="I38">
-        <v>0.362458</v>
-      </c>
-      <c r="J38">
-        <v>3.1199999999999999E-4</v>
-      </c>
-      <c r="K38">
-        <v>0</v>
-      </c>
-      <c r="L38">
-        <v>5.0629999999999998E-3</v>
-      </c>
-      <c r="M38">
-        <v>9.0449999999999992E-3</v>
-      </c>
-      <c r="N38">
-        <v>6.1139999999999996E-3</v>
-      </c>
-      <c r="O38">
+      <c r="I38" s="1">
+        <v>42.347999999999999</v>
+      </c>
+      <c r="J38" s="1">
+        <v>69.569999999999993</v>
+      </c>
+      <c r="K38" s="1">
+        <v>1.6439999999999999</v>
+      </c>
+      <c r="L38" s="1">
+        <v>1.1439999999999999</v>
+      </c>
+      <c r="M38" s="1">
+        <v>9.4689999999999994</v>
+      </c>
+      <c r="N38" s="1">
+        <v>59.847000000000001</v>
+      </c>
+      <c r="O38" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B39" t="s">
         <v>40</v>
@@ -2351,31 +2361,31 @@
       <c r="H39">
         <v>2</v>
       </c>
-      <c r="I39">
-        <v>0.302568</v>
-      </c>
-      <c r="J39">
-        <v>3.3100000000000002E-4</v>
-      </c>
-      <c r="K39">
-        <v>0</v>
-      </c>
-      <c r="L39">
-        <v>4.8949999999999992E-3</v>
-      </c>
-      <c r="M39">
-        <v>7.6540000000000002E-3</v>
-      </c>
-      <c r="N39">
-        <v>1.5247999999999999E-2</v>
-      </c>
-      <c r="O39">
-        <v>2.0999999999999998E-4</v>
+      <c r="I39" s="1">
+        <v>44.234999999999999</v>
+      </c>
+      <c r="J39" s="1">
+        <v>66.677999999999997</v>
+      </c>
+      <c r="K39" s="1">
+        <v>1.2669999999999999</v>
+      </c>
+      <c r="L39" s="1">
+        <v>1.0980000000000001</v>
+      </c>
+      <c r="M39" s="1">
+        <v>8.9670000000000005</v>
+      </c>
+      <c r="N39" s="1">
+        <v>66.578000000000003</v>
+      </c>
+      <c r="O39" s="1">
+        <v>0.1</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B40" t="s">
         <v>40</v>
@@ -2398,31 +2408,31 @@
       <c r="H40">
         <v>2</v>
       </c>
-      <c r="I40">
-        <v>0.34168999999999999</v>
-      </c>
-      <c r="J40">
-        <v>2.8699999999999998E-4</v>
-      </c>
-      <c r="K40">
-        <v>0</v>
-      </c>
-      <c r="L40">
-        <v>5.4359999999999999E-3</v>
-      </c>
-      <c r="M40">
-        <v>8.5789999999999998E-3</v>
-      </c>
-      <c r="N40">
-        <v>1.3578E-2</v>
-      </c>
-      <c r="O40">
-        <v>1.4000000000000001E-4</v>
+      <c r="I40" s="1">
+        <v>39.578000000000003</v>
+      </c>
+      <c r="J40" s="1">
+        <v>72.650000000000006</v>
+      </c>
+      <c r="K40" s="1">
+        <v>1.35</v>
+      </c>
+      <c r="L40" s="1">
+        <v>1.2669999999999999</v>
+      </c>
+      <c r="M40" s="1">
+        <v>8.6639999999999997</v>
+      </c>
+      <c r="N40" s="1">
+        <v>62.353999999999999</v>
+      </c>
+      <c r="O40" s="1">
+        <v>0.09</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="B41" t="s">
         <v>40</v>
@@ -2440,36 +2450,36 @@
         <v>1</v>
       </c>
       <c r="G41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I41">
-        <v>2.466421</v>
+        <v>34.427999999999997</v>
       </c>
       <c r="J41">
-        <v>5.1143000000000001E-2</v>
+        <v>45.674999999999997</v>
       </c>
       <c r="K41">
-        <v>7.4489999999999999E-3</v>
+        <v>2.57</v>
       </c>
       <c r="L41">
-        <v>1.2539999999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="M41">
-        <v>7.2259999999999998E-3</v>
+        <v>4.0650000000000004</v>
       </c>
       <c r="N41">
-        <v>3.2753999999999998E-2</v>
+        <v>45.783999999999999</v>
       </c>
       <c r="O41">
-        <v>1.3375E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="B42" t="s">
         <v>40</v>
@@ -2487,36 +2497,36 @@
         <v>1</v>
       </c>
       <c r="G42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I42">
-        <v>2.3455599999999999</v>
+        <v>34.950000000000003</v>
       </c>
       <c r="J42">
-        <v>5.0650000000000001E-2</v>
+        <v>39.51</v>
       </c>
       <c r="K42">
-        <v>7.1500000000000001E-3</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="L42">
-        <v>1.268E-3</v>
+        <v>0.1</v>
       </c>
       <c r="M42">
-        <v>7.1159999999999999E-3</v>
+        <v>3.56</v>
       </c>
       <c r="N42">
-        <v>3.168E-2</v>
+        <v>39.909999999999997</v>
       </c>
       <c r="O42">
-        <v>1.567E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>40</v>
@@ -2534,42 +2544,42 @@
         <v>1</v>
       </c>
       <c r="G43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I43">
-        <v>2.1595800000000001</v>
+        <v>35.020000000000003</v>
       </c>
       <c r="J43">
-        <v>5.3249999999999999E-2</v>
+        <v>37.65</v>
       </c>
       <c r="K43">
-        <v>6.9800000000000001E-3</v>
+        <v>3.56</v>
       </c>
       <c r="L43">
-        <v>1.2470000000000001E-3</v>
+        <v>0.12</v>
       </c>
       <c r="M43">
-        <v>6.9979999999999999E-3</v>
+        <v>3.81</v>
       </c>
       <c r="N43">
-        <v>3.2570000000000002E-2</v>
+        <v>38.97</v>
       </c>
       <c r="O43">
-        <v>1.4590000000000001E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B44" t="s">
         <v>40</v>
       </c>
       <c r="C44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D44">
         <v>2020</v>
@@ -2586,37 +2596,37 @@
       <c r="H44">
         <v>2</v>
       </c>
-      <c r="I44">
-        <v>0.38453300000000001</v>
-      </c>
-      <c r="J44">
-        <v>3.4442E-2</v>
-      </c>
-      <c r="K44">
-        <v>0</v>
-      </c>
-      <c r="L44">
-        <v>0</v>
-      </c>
-      <c r="M44">
-        <v>1.9906E-2</v>
-      </c>
-      <c r="N44">
-        <v>0.105222</v>
-      </c>
-      <c r="O44">
-        <v>1.0872999999999999E-2</v>
+      <c r="I44" s="1">
+        <v>362.45800000000003</v>
+      </c>
+      <c r="J44" s="1">
+        <v>0.312</v>
+      </c>
+      <c r="K44" s="1">
+        <v>0</v>
+      </c>
+      <c r="L44" s="1">
+        <v>5.0629999999999997</v>
+      </c>
+      <c r="M44" s="1">
+        <v>9.0449999999999999</v>
+      </c>
+      <c r="N44" s="1">
+        <v>6.1139999999999999</v>
+      </c>
+      <c r="O44" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B45" t="s">
         <v>40</v>
       </c>
       <c r="C45" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D45">
         <v>2020</v>
@@ -2633,37 +2643,37 @@
       <c r="H45">
         <v>2</v>
       </c>
-      <c r="I45">
-        <v>0.17969200000000002</v>
-      </c>
-      <c r="J45">
-        <v>3.024E-2</v>
-      </c>
-      <c r="K45">
-        <v>3.3809999999999999E-3</v>
-      </c>
-      <c r="L45">
-        <v>3.4120000000000001E-3</v>
-      </c>
-      <c r="M45">
-        <v>2.1222000000000001E-2</v>
-      </c>
-      <c r="N45">
-        <v>7.4089000000000002E-2</v>
-      </c>
-      <c r="O45">
-        <v>6.2500000000000003E-3</v>
+      <c r="I45" s="1">
+        <v>302.56799999999998</v>
+      </c>
+      <c r="J45" s="1">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="K45" s="1">
+        <v>0</v>
+      </c>
+      <c r="L45" s="1">
+        <v>4.8949999999999996</v>
+      </c>
+      <c r="M45" s="1">
+        <v>7.6539999999999999</v>
+      </c>
+      <c r="N45" s="1">
+        <v>15.247999999999999</v>
+      </c>
+      <c r="O45" s="1">
+        <v>0.21</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B46" t="s">
         <v>40</v>
       </c>
       <c r="C46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D46">
         <v>2020</v>
@@ -2680,31 +2690,31 @@
       <c r="H46">
         <v>2</v>
       </c>
-      <c r="I46">
-        <v>0.59855899999999995</v>
-      </c>
-      <c r="J46">
-        <v>4.2158000000000001E-2</v>
-      </c>
-      <c r="K46">
-        <v>3.2229999999999997E-3</v>
-      </c>
-      <c r="L46">
-        <v>1.1999999999999999E-3</v>
-      </c>
-      <c r="M46">
-        <v>9.1339999999999998E-3</v>
-      </c>
-      <c r="N46">
-        <v>4.6906999999999997E-2</v>
-      </c>
-      <c r="O46">
-        <v>9.0989999999999994E-3</v>
+      <c r="I46" s="1">
+        <v>341.69</v>
+      </c>
+      <c r="J46" s="1">
+        <v>0.28699999999999998</v>
+      </c>
+      <c r="K46" s="1">
+        <v>0</v>
+      </c>
+      <c r="L46" s="1">
+        <v>5.4359999999999999</v>
+      </c>
+      <c r="M46" s="1">
+        <v>8.5790000000000006</v>
+      </c>
+      <c r="N46" s="1">
+        <v>13.577999999999999</v>
+      </c>
+      <c r="O46" s="1">
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B47" t="s">
         <v>40</v>
@@ -2727,31 +2737,31 @@
       <c r="H47">
         <v>2</v>
       </c>
-      <c r="I47">
-        <v>0.20813499999999999</v>
-      </c>
-      <c r="J47">
-        <v>4.3252000000000006E-2</v>
-      </c>
-      <c r="K47">
-        <v>0</v>
-      </c>
-      <c r="L47">
-        <v>1.5428000000000001E-2</v>
-      </c>
-      <c r="M47">
-        <v>1.728E-2</v>
-      </c>
-      <c r="N47">
-        <v>4.7971E-2</v>
-      </c>
-      <c r="O47">
-        <v>0</v>
+      <c r="I47" s="1">
+        <v>2466.4209999999998</v>
+      </c>
+      <c r="J47" s="1">
+        <v>51.143000000000001</v>
+      </c>
+      <c r="K47" s="1">
+        <v>7.4489999999999998</v>
+      </c>
+      <c r="L47" s="1">
+        <v>1.254</v>
+      </c>
+      <c r="M47" s="1">
+        <v>7.226</v>
+      </c>
+      <c r="N47" s="1">
+        <v>32.753999999999998</v>
+      </c>
+      <c r="O47" s="1">
+        <v>13.375</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B48" t="s">
         <v>40</v>
@@ -2774,31 +2784,31 @@
       <c r="H48">
         <v>2</v>
       </c>
-      <c r="I48">
-        <v>0.20915</v>
-      </c>
-      <c r="J48">
-        <v>4.1250000000000002E-2</v>
-      </c>
-      <c r="K48">
-        <v>2.5000000000000001E-4</v>
-      </c>
-      <c r="L48">
-        <v>1.6570000000000001E-2</v>
-      </c>
-      <c r="M48">
-        <v>1.6980000000000002E-2</v>
-      </c>
-      <c r="N48">
-        <v>4.9239999999999999E-2</v>
-      </c>
-      <c r="O48">
-        <v>0</v>
+      <c r="I48" s="1">
+        <v>2345.56</v>
+      </c>
+      <c r="J48" s="1">
+        <v>50.65</v>
+      </c>
+      <c r="K48" s="1">
+        <v>7.15</v>
+      </c>
+      <c r="L48" s="1">
+        <v>1.268</v>
+      </c>
+      <c r="M48" s="1">
+        <v>7.1159999999999997</v>
+      </c>
+      <c r="N48" s="1">
+        <v>31.68</v>
+      </c>
+      <c r="O48" s="1">
+        <v>15.67</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B49" t="s">
         <v>40</v>
@@ -2821,37 +2831,37 @@
       <c r="H49">
         <v>2</v>
       </c>
-      <c r="I49">
-        <v>0.20557</v>
-      </c>
-      <c r="J49">
-        <v>4.4289999999999996E-2</v>
-      </c>
-      <c r="K49">
-        <v>1.1999999999999999E-4</v>
-      </c>
-      <c r="L49">
-        <v>1.712E-2</v>
-      </c>
-      <c r="M49">
-        <v>1.8539999999999997E-2</v>
-      </c>
-      <c r="N49">
-        <v>5.5229999999999994E-2</v>
-      </c>
-      <c r="O49">
-        <v>0</v>
+      <c r="I49" s="1">
+        <v>2159.58</v>
+      </c>
+      <c r="J49" s="1">
+        <v>53.25</v>
+      </c>
+      <c r="K49" s="1">
+        <v>6.98</v>
+      </c>
+      <c r="L49" s="1">
+        <v>1.2470000000000001</v>
+      </c>
+      <c r="M49" s="1">
+        <v>6.9980000000000002</v>
+      </c>
+      <c r="N49" s="1">
+        <v>32.57</v>
+      </c>
+      <c r="O49" s="1">
+        <v>14.59</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B50" t="s">
         <v>40</v>
       </c>
       <c r="C50" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D50">
         <v>2020</v>
@@ -2868,37 +2878,37 @@
       <c r="H50">
         <v>2</v>
       </c>
-      <c r="I50">
-        <v>0.19778299999999999</v>
-      </c>
-      <c r="J50">
-        <v>5.2316000000000001E-2</v>
-      </c>
-      <c r="K50">
-        <v>0</v>
-      </c>
-      <c r="L50">
-        <v>5.3249999999999999E-3</v>
-      </c>
-      <c r="M50">
-        <v>7.4869999999999997E-3</v>
-      </c>
-      <c r="N50">
-        <v>1.1182000000000001E-2</v>
-      </c>
-      <c r="O50">
-        <v>1.6899999999999999E-3</v>
+      <c r="I50" s="1">
+        <v>384.53300000000002</v>
+      </c>
+      <c r="J50" s="1">
+        <v>34.442</v>
+      </c>
+      <c r="K50" s="1">
+        <v>0</v>
+      </c>
+      <c r="L50" s="1">
+        <v>0</v>
+      </c>
+      <c r="M50" s="1">
+        <v>19.905999999999999</v>
+      </c>
+      <c r="N50" s="1">
+        <v>105.22199999999999</v>
+      </c>
+      <c r="O50" s="1">
+        <v>10.872999999999999</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B51" t="s">
         <v>40</v>
       </c>
       <c r="C51" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D51">
         <v>2020</v>
@@ -2915,37 +2925,37 @@
       <c r="H51">
         <v>2</v>
       </c>
-      <c r="I51">
-        <v>0.21029</v>
-      </c>
-      <c r="J51">
-        <v>5.0290000000000001E-2</v>
-      </c>
-      <c r="K51">
-        <v>0</v>
-      </c>
-      <c r="L51">
-        <v>2.98E-3</v>
-      </c>
-      <c r="M51">
-        <v>7.1200000000000005E-3</v>
-      </c>
-      <c r="N51">
-        <v>1.098E-2</v>
-      </c>
-      <c r="O51">
-        <v>1.57E-3</v>
+      <c r="I51" s="1">
+        <v>179.69200000000001</v>
+      </c>
+      <c r="J51" s="1">
+        <v>30.24</v>
+      </c>
+      <c r="K51" s="1">
+        <v>3.3809999999999998</v>
+      </c>
+      <c r="L51" s="1">
+        <v>3.4119999999999999</v>
+      </c>
+      <c r="M51" s="1">
+        <v>21.222000000000001</v>
+      </c>
+      <c r="N51" s="1">
+        <v>74.088999999999999</v>
+      </c>
+      <c r="O51" s="1">
+        <v>6.25</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B52" t="s">
         <v>40</v>
       </c>
       <c r="C52" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D52">
         <v>2020</v>
@@ -2962,31 +2972,31 @@
       <c r="H52">
         <v>2</v>
       </c>
-      <c r="I52">
-        <v>0.20118</v>
-      </c>
-      <c r="J52">
-        <v>4.9779999999999998E-2</v>
-      </c>
-      <c r="K52">
-        <v>0</v>
-      </c>
-      <c r="L52">
-        <v>4.8700000000000002E-3</v>
-      </c>
-      <c r="M52">
-        <v>6.9800000000000001E-3</v>
-      </c>
-      <c r="N52">
-        <v>1.2160000000000001E-2</v>
-      </c>
-      <c r="O52">
-        <v>1.15E-3</v>
+      <c r="I52" s="1">
+        <v>598.55899999999997</v>
+      </c>
+      <c r="J52" s="1">
+        <v>42.158000000000001</v>
+      </c>
+      <c r="K52" s="1">
+        <v>3.2229999999999999</v>
+      </c>
+      <c r="L52" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="M52" s="1">
+        <v>9.1340000000000003</v>
+      </c>
+      <c r="N52" s="1">
+        <v>46.906999999999996</v>
+      </c>
+      <c r="O52" s="1">
+        <v>9.0990000000000002</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B53" t="s">
         <v>40</v>
@@ -3004,36 +3014,36 @@
         <v>1</v>
       </c>
       <c r="G53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I53">
-        <v>0.21294099999999999</v>
+        <v>270.702</v>
       </c>
       <c r="J53">
-        <v>5.4079000000000002E-2</v>
+        <v>42.783999999999999</v>
       </c>
       <c r="K53">
         <v>0</v>
       </c>
       <c r="L53">
-        <v>3.6829999999999996E-3</v>
+        <v>2.2040000000000002</v>
       </c>
       <c r="M53">
-        <v>9.1430000000000001E-3</v>
+        <v>6.992</v>
       </c>
       <c r="N53">
-        <v>4.9917000000000003E-2</v>
+        <v>74.423000000000002</v>
       </c>
       <c r="O53">
-        <v>2.6949999999999999E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B54" t="s">
         <v>40</v>
@@ -3051,36 +3061,36 @@
         <v>1</v>
       </c>
       <c r="G54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I54">
-        <v>0.21356</v>
+        <v>265.25</v>
       </c>
       <c r="J54">
-        <v>5.5039999999999999E-2</v>
+        <v>41.26</v>
       </c>
       <c r="K54">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="L54">
-        <v>3.9700000000000004E-3</v>
+        <v>1.98</v>
       </c>
       <c r="M54">
-        <v>8.9779999999999999E-3</v>
+        <v>7.68</v>
       </c>
       <c r="N54">
-        <v>5.0256000000000002E-2</v>
+        <v>77.86</v>
       </c>
       <c r="O54">
-        <v>2.9870000000000001E-3</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B55" t="s">
         <v>40</v>
@@ -3098,36 +3108,36 @@
         <v>1</v>
       </c>
       <c r="G55">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H55">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I55">
-        <v>0.21415799999999999</v>
+        <v>273.56</v>
       </c>
       <c r="J55">
-        <v>5.4579999999999997E-2</v>
+        <v>43.87</v>
       </c>
       <c r="K55">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="L55">
-        <v>4.0199999999999993E-3</v>
+        <v>2.34</v>
       </c>
       <c r="M55">
-        <v>9.0153999999999998E-3</v>
+        <v>6.98</v>
       </c>
       <c r="N55">
-        <v>4.9877999999999999E-2</v>
+        <v>81.239999999999995</v>
       </c>
       <c r="O55">
-        <v>3.0139999999999998E-3</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B56" t="s">
         <v>40</v>
@@ -3151,22 +3161,22 @@
         <v>2</v>
       </c>
       <c r="I56">
-        <v>0.18037299999999998</v>
+        <v>208.13499999999999</v>
       </c>
       <c r="J56">
-        <v>8.0380999999999994E-2</v>
+        <v>43.252000000000002</v>
       </c>
       <c r="K56">
         <v>0</v>
       </c>
       <c r="L56">
-        <v>3.6779999999999998E-3</v>
+        <v>15.428000000000001</v>
       </c>
       <c r="M56">
-        <v>8.1569999999999993E-3</v>
+        <v>17.28</v>
       </c>
       <c r="N56">
-        <v>0.10352800000000001</v>
+        <v>47.970999999999997</v>
       </c>
       <c r="O56">
         <v>0</v>
@@ -3174,7 +3184,7 @@
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B57" t="s">
         <v>40</v>
@@ -3198,30 +3208,30 @@
         <v>2</v>
       </c>
       <c r="I57">
-        <v>0.18357400000000001</v>
+        <v>209.15</v>
       </c>
       <c r="J57">
-        <v>8.0268000000000006E-2</v>
+        <v>41.25</v>
       </c>
       <c r="K57">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="L57">
-        <v>3.8969999999999999E-3</v>
+        <v>16.57</v>
       </c>
       <c r="M57">
-        <v>7.9679999999999994E-3</v>
+        <v>16.98</v>
       </c>
       <c r="N57">
-        <v>0.10026500000000001</v>
+        <v>49.24</v>
       </c>
       <c r="O57">
-        <v>1.11E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B58" t="s">
         <v>40</v>
@@ -3245,30 +3255,30 @@
         <v>2</v>
       </c>
       <c r="I58">
-        <v>0.179257</v>
+        <v>205.57</v>
       </c>
       <c r="J58">
-        <v>7.7997999999999998E-2</v>
+        <v>44.29</v>
       </c>
       <c r="K58">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="L58">
-        <v>3.754E-3</v>
+        <v>17.12</v>
       </c>
       <c r="M58">
-        <v>8.1950000000000009E-3</v>
+        <v>18.54</v>
       </c>
       <c r="N58">
-        <v>0.10535700000000001</v>
+        <v>55.23</v>
       </c>
       <c r="O58">
-        <v>1.0899999999999999E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B59" t="s">
         <v>40</v>
@@ -3292,30 +3302,30 @@
         <v>2</v>
       </c>
       <c r="I59">
-        <v>0.19968</v>
+        <v>197.78299999999999</v>
       </c>
       <c r="J59">
-        <v>2.9579999999999999E-2</v>
+        <v>52.316000000000003</v>
       </c>
       <c r="K59">
-        <v>2.9420000000000002E-3</v>
+        <v>0</v>
       </c>
       <c r="L59">
-        <v>1.1E-4</v>
+        <v>5.3250000000000002</v>
       </c>
       <c r="M59">
-        <v>3.6853000000000004E-2</v>
+        <v>7.4870000000000001</v>
       </c>
       <c r="N59">
-        <v>0.24540799999999999</v>
+        <v>11.182</v>
       </c>
       <c r="O59">
-        <v>2.6840000000000002E-3</v>
+        <v>1.69</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B60" t="s">
         <v>40</v>
@@ -3339,30 +3349,30 @@
         <v>2</v>
       </c>
       <c r="I60">
-        <v>0.36155100000000001</v>
+        <v>210.29</v>
       </c>
       <c r="J60">
-        <v>3.8670999999999997E-2</v>
+        <v>50.29</v>
       </c>
       <c r="K60">
-        <v>1.258E-3</v>
+        <v>0</v>
       </c>
       <c r="L60">
-        <v>0</v>
+        <v>2.98</v>
       </c>
       <c r="M60">
-        <v>3.8308999999999996E-2</v>
+        <v>7.12</v>
       </c>
       <c r="N60">
-        <v>0.20971799999999999</v>
+        <v>10.98</v>
       </c>
       <c r="O60">
-        <v>3.1402999999999999E-3</v>
+        <v>1.57</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B61" t="s">
         <v>40</v>
@@ -3386,30 +3396,30 @@
         <v>2</v>
       </c>
       <c r="I61">
-        <v>0.32958300000000001</v>
+        <v>201.18</v>
       </c>
       <c r="J61">
-        <v>2.1260000000000001E-2</v>
+        <v>49.78</v>
       </c>
       <c r="K61">
-        <v>3.6649999999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="L61">
-        <v>1E-4</v>
+        <v>4.87</v>
       </c>
       <c r="M61">
-        <v>3.5682000000000005E-2</v>
+        <v>6.98</v>
       </c>
       <c r="N61">
-        <v>0.224357</v>
+        <v>12.16</v>
       </c>
       <c r="O61">
-        <v>2.8889999999999996E-3</v>
+        <v>1.1499999999999999</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B62" t="s">
         <v>40</v>
@@ -3433,30 +3443,30 @@
         <v>2</v>
       </c>
       <c r="I62">
-        <v>2.6257000000000003E-2</v>
+        <v>212.941</v>
       </c>
       <c r="J62">
-        <v>6.1751E-2</v>
+        <v>54.079000000000001</v>
       </c>
       <c r="K62">
         <v>0</v>
       </c>
       <c r="L62">
-        <v>1.9479999999999999E-3</v>
+        <v>3.6829999999999998</v>
       </c>
       <c r="M62">
-        <v>8.966E-3</v>
+        <v>9.1430000000000007</v>
       </c>
       <c r="N62">
-        <v>3.0282E-2</v>
+        <v>49.917000000000002</v>
       </c>
       <c r="O62">
-        <v>3.5270000000000002E-3</v>
+        <v>2.6949999999999998</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B63" t="s">
         <v>40</v>
@@ -3480,30 +3490,30 @@
         <v>2</v>
       </c>
       <c r="I63">
-        <v>2.6456E-2</v>
+        <v>213.56</v>
       </c>
       <c r="J63">
-        <v>6.3543000000000002E-2</v>
+        <v>55.04</v>
       </c>
       <c r="K63">
         <v>0</v>
       </c>
       <c r="L63">
-        <v>1.8859999999999999E-3</v>
+        <v>3.97</v>
       </c>
       <c r="M63">
-        <v>9.2639999999999997E-3</v>
+        <v>8.9779999999999998</v>
       </c>
       <c r="N63">
-        <v>3.1022999999999998E-2</v>
+        <v>50.256</v>
       </c>
       <c r="O63">
-        <v>3.6120000000000002E-3</v>
+        <v>2.9870000000000001</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B64" t="s">
         <v>40</v>
@@ -3527,25 +3537,448 @@
         <v>2</v>
       </c>
       <c r="I64">
-        <v>2.5874999999999999E-2</v>
+        <v>214.15799999999999</v>
       </c>
       <c r="J64">
-        <v>6.3140000000000002E-2</v>
+        <v>54.58</v>
       </c>
       <c r="K64">
         <v>0</v>
       </c>
       <c r="L64">
-        <v>1.9119999999999999E-3</v>
+        <v>4.0199999999999996</v>
       </c>
       <c r="M64">
-        <v>9.1039999999999992E-3</v>
+        <v>9.0153999999999996</v>
       </c>
       <c r="N64">
-        <v>3.0824999999999998E-2</v>
+        <v>49.878</v>
       </c>
       <c r="O64">
-        <v>3.5539999999999999E-3</v>
+        <v>3.0139999999999998</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>28</v>
+      </c>
+      <c r="B65" t="s">
+        <v>40</v>
+      </c>
+      <c r="C65" t="s">
+        <v>37</v>
+      </c>
+      <c r="D65">
+        <v>2020</v>
+      </c>
+      <c r="E65" t="s">
+        <v>8</v>
+      </c>
+      <c r="F65">
+        <v>1</v>
+      </c>
+      <c r="G65">
+        <v>2</v>
+      </c>
+      <c r="H65">
+        <v>2</v>
+      </c>
+      <c r="I65" s="1">
+        <v>180.37299999999999</v>
+      </c>
+      <c r="J65" s="1">
+        <v>80.381</v>
+      </c>
+      <c r="K65" s="1">
+        <v>0</v>
+      </c>
+      <c r="L65" s="1">
+        <v>3.6779999999999999</v>
+      </c>
+      <c r="M65" s="1">
+        <v>8.157</v>
+      </c>
+      <c r="N65" s="1">
+        <v>103.52800000000001</v>
+      </c>
+      <c r="O65" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>28</v>
+      </c>
+      <c r="B66" t="s">
+        <v>40</v>
+      </c>
+      <c r="C66" t="s">
+        <v>37</v>
+      </c>
+      <c r="D66">
+        <v>2020</v>
+      </c>
+      <c r="E66" t="s">
+        <v>9</v>
+      </c>
+      <c r="F66">
+        <v>1</v>
+      </c>
+      <c r="G66">
+        <v>2</v>
+      </c>
+      <c r="H66">
+        <v>2</v>
+      </c>
+      <c r="I66" s="1">
+        <v>183.57400000000001</v>
+      </c>
+      <c r="J66" s="1">
+        <v>80.268000000000001</v>
+      </c>
+      <c r="K66" s="1">
+        <v>0</v>
+      </c>
+      <c r="L66" s="1">
+        <v>3.8969999999999998</v>
+      </c>
+      <c r="M66" s="1">
+        <v>7.968</v>
+      </c>
+      <c r="N66" s="1">
+        <v>100.265</v>
+      </c>
+      <c r="O66" s="1">
+        <v>0.111</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>28</v>
+      </c>
+      <c r="B67" t="s">
+        <v>40</v>
+      </c>
+      <c r="C67" t="s">
+        <v>37</v>
+      </c>
+      <c r="D67">
+        <v>2020</v>
+      </c>
+      <c r="E67" t="s">
+        <v>10</v>
+      </c>
+      <c r="F67">
+        <v>1</v>
+      </c>
+      <c r="G67">
+        <v>2</v>
+      </c>
+      <c r="H67">
+        <v>2</v>
+      </c>
+      <c r="I67" s="1">
+        <v>179.25700000000001</v>
+      </c>
+      <c r="J67" s="1">
+        <v>77.998000000000005</v>
+      </c>
+      <c r="K67" s="1">
+        <v>0</v>
+      </c>
+      <c r="L67" s="1">
+        <v>3.754</v>
+      </c>
+      <c r="M67" s="1">
+        <v>8.1950000000000003</v>
+      </c>
+      <c r="N67" s="1">
+        <v>105.357</v>
+      </c>
+      <c r="O67" s="1">
+        <v>0.109</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>29</v>
+      </c>
+      <c r="B68" t="s">
+        <v>40</v>
+      </c>
+      <c r="C68" t="s">
+        <v>37</v>
+      </c>
+      <c r="D68">
+        <v>2020</v>
+      </c>
+      <c r="E68" t="s">
+        <v>8</v>
+      </c>
+      <c r="F68">
+        <v>1</v>
+      </c>
+      <c r="G68">
+        <v>2</v>
+      </c>
+      <c r="H68">
+        <v>2</v>
+      </c>
+      <c r="I68">
+        <v>199.68</v>
+      </c>
+      <c r="J68">
+        <v>29.58</v>
+      </c>
+      <c r="K68">
+        <v>2.9420000000000002</v>
+      </c>
+      <c r="L68">
+        <v>0.11</v>
+      </c>
+      <c r="M68">
+        <v>36.853000000000002</v>
+      </c>
+      <c r="N68">
+        <v>245.40799999999999</v>
+      </c>
+      <c r="O68">
+        <v>2.6840000000000002</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>29</v>
+      </c>
+      <c r="B69" t="s">
+        <v>40</v>
+      </c>
+      <c r="C69" t="s">
+        <v>37</v>
+      </c>
+      <c r="D69">
+        <v>2020</v>
+      </c>
+      <c r="E69" t="s">
+        <v>9</v>
+      </c>
+      <c r="F69">
+        <v>1</v>
+      </c>
+      <c r="G69">
+        <v>2</v>
+      </c>
+      <c r="H69">
+        <v>2</v>
+      </c>
+      <c r="I69">
+        <v>361.55099999999999</v>
+      </c>
+      <c r="J69">
+        <v>38.670999999999999</v>
+      </c>
+      <c r="K69">
+        <v>1.258</v>
+      </c>
+      <c r="L69">
+        <v>0</v>
+      </c>
+      <c r="M69">
+        <v>38.308999999999997</v>
+      </c>
+      <c r="N69">
+        <v>209.71799999999999</v>
+      </c>
+      <c r="O69">
+        <v>3.1402999999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>29</v>
+      </c>
+      <c r="B70" t="s">
+        <v>40</v>
+      </c>
+      <c r="C70" t="s">
+        <v>37</v>
+      </c>
+      <c r="D70">
+        <v>2020</v>
+      </c>
+      <c r="E70" t="s">
+        <v>10</v>
+      </c>
+      <c r="F70">
+        <v>1</v>
+      </c>
+      <c r="G70">
+        <v>2</v>
+      </c>
+      <c r="H70">
+        <v>2</v>
+      </c>
+      <c r="I70">
+        <v>329.58300000000003</v>
+      </c>
+      <c r="J70">
+        <v>21.26</v>
+      </c>
+      <c r="K70">
+        <v>3.665</v>
+      </c>
+      <c r="L70">
+        <v>0.1</v>
+      </c>
+      <c r="M70">
+        <v>35.682000000000002</v>
+      </c>
+      <c r="N70">
+        <v>224.357</v>
+      </c>
+      <c r="O70">
+        <v>2.8889999999999998</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>30</v>
+      </c>
+      <c r="B71" t="s">
+        <v>40</v>
+      </c>
+      <c r="C71" t="s">
+        <v>37</v>
+      </c>
+      <c r="D71">
+        <v>2020</v>
+      </c>
+      <c r="E71" t="s">
+        <v>8</v>
+      </c>
+      <c r="F71">
+        <v>1</v>
+      </c>
+      <c r="G71">
+        <v>2</v>
+      </c>
+      <c r="H71">
+        <v>2</v>
+      </c>
+      <c r="I71" s="1">
+        <v>26.257000000000001</v>
+      </c>
+      <c r="J71" s="1">
+        <v>61.750999999999998</v>
+      </c>
+      <c r="K71" s="1">
+        <v>0</v>
+      </c>
+      <c r="L71" s="1">
+        <v>1.948</v>
+      </c>
+      <c r="M71" s="1">
+        <v>8.9659999999999993</v>
+      </c>
+      <c r="N71" s="1">
+        <v>30.282</v>
+      </c>
+      <c r="O71" s="1">
+        <v>3.5270000000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>30</v>
+      </c>
+      <c r="B72" t="s">
+        <v>40</v>
+      </c>
+      <c r="C72" t="s">
+        <v>37</v>
+      </c>
+      <c r="D72">
+        <v>2020</v>
+      </c>
+      <c r="E72" t="s">
+        <v>9</v>
+      </c>
+      <c r="F72">
+        <v>1</v>
+      </c>
+      <c r="G72">
+        <v>2</v>
+      </c>
+      <c r="H72">
+        <v>2</v>
+      </c>
+      <c r="I72" s="1">
+        <v>26.456</v>
+      </c>
+      <c r="J72" s="1">
+        <v>63.542999999999999</v>
+      </c>
+      <c r="K72" s="1">
+        <v>0</v>
+      </c>
+      <c r="L72" s="1">
+        <v>1.8859999999999999</v>
+      </c>
+      <c r="M72" s="1">
+        <v>9.2639999999999993</v>
+      </c>
+      <c r="N72" s="1">
+        <v>31.023</v>
+      </c>
+      <c r="O72" s="1">
+        <v>3.6120000000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>30</v>
+      </c>
+      <c r="B73" t="s">
+        <v>40</v>
+      </c>
+      <c r="C73" t="s">
+        <v>37</v>
+      </c>
+      <c r="D73">
+        <v>2020</v>
+      </c>
+      <c r="E73" t="s">
+        <v>10</v>
+      </c>
+      <c r="F73">
+        <v>1</v>
+      </c>
+      <c r="G73">
+        <v>2</v>
+      </c>
+      <c r="H73">
+        <v>2</v>
+      </c>
+      <c r="I73" s="1">
+        <v>25.875</v>
+      </c>
+      <c r="J73" s="1">
+        <v>63.14</v>
+      </c>
+      <c r="K73" s="1">
+        <v>0</v>
+      </c>
+      <c r="L73" s="1">
+        <v>1.9119999999999999</v>
+      </c>
+      <c r="M73" s="1">
+        <v>9.1039999999999992</v>
+      </c>
+      <c r="N73" s="1">
+        <v>30.824999999999999</v>
+      </c>
+      <c r="O73" s="1">
+        <v>3.5539999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>